<commit_message>
add response initialization to 0 to avoid response obj missing some attributes
</commit_message>
<xml_diff>
--- a/results/MQA-Metrics-Report.xlsx
+++ b/results/MQA-Metrics-Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\BeOpen\mqa-scoring\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85143A4-1125-4630-ACB7-60CBB25FED92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E4B71-BE8E-4F0A-83CD-2CAF3ECF38FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6645" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-3735" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERSTAT" sheetId="176" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>INTERSTAT</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>TOT:</t>
+  </si>
+  <si>
+    <t>shacl</t>
   </si>
 </sst>
 </file>
@@ -541,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,6 +1123,9 @@
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="D85" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">

</xml_diff>